<commit_message>
cuentas anulacion y esas weas
</commit_message>
<xml_diff>
--- a/E2ESIT.xlsx
+++ b/E2ESIT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Altas y Nominacion" sheetId="8" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="191">
   <si>
     <t>N.º Documento</t>
   </si>
@@ -236,9 +236,6 @@
     <t>Newton</t>
   </si>
   <si>
-    <t>22222001</t>
-  </si>
-  <si>
     <t>123</t>
   </si>
   <si>
@@ -585,6 +582,18 @@
   </si>
   <si>
     <t>1164786972</t>
+  </si>
+  <si>
+    <t>19006577</t>
+  </si>
+  <si>
+    <t>59885133</t>
+  </si>
+  <si>
+    <t>Gestion Anulacion de venta</t>
+  </si>
+  <si>
+    <t>Anulacion De Venta</t>
   </si>
 </sst>
 </file>
@@ -1154,7 +1163,7 @@
   <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1176,7 +1185,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1206,46 +1215,46 @@
         <v>16</v>
       </c>
       <c r="K1" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>148</v>
-      </c>
       <c r="N1" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="O1" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="P1" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="R1" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="Q1" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="R1" s="11" t="s">
+      <c r="S1" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="T1" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="T1" s="11" t="s">
+      <c r="U1" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="V1" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="W1" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="W1" s="11" t="s">
-        <v>116</v>
-      </c>
       <c r="X1" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
@@ -1402,7 +1411,7 @@
         <v>52</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C5" t="s">
         <v>56</v>
@@ -1438,19 +1447,19 @@
         <v>37</v>
       </c>
       <c r="N5" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="O5" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P5" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q5" s="18" t="s">
         <v>44</v>
       </c>
       <c r="R5" s="25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="S5" s="32" t="s">
         <v>41</v>
@@ -1468,12 +1477,12 @@
         <v>69</v>
       </c>
       <c r="X5" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:26" s="46" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>0</v>
@@ -1482,19 +1491,19 @@
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>110</v>
-      </c>
       <c r="G6" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -1517,28 +1526,28 @@
     </row>
     <row r="7" spans="1:26" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A7" s="53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" s="55" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C7" s="40" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F7" s="32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G7" s="32" t="s">
         <v>44</v>
       </c>
       <c r="H7" s="32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I7" s="31"/>
       <c r="J7" s="31"/>
@@ -1554,7 +1563,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="55" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C8" s="40" t="s">
         <v>2</v>
@@ -1573,7 +1582,7 @@
     </row>
     <row r="9" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>0</v>
@@ -1597,7 +1606,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>15</v>
@@ -1606,46 +1615,46 @@
         <v>16</v>
       </c>
       <c r="L9" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="M9" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="N9" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="N9" s="3" t="s">
-        <v>148</v>
-      </c>
       <c r="O9" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="P9" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="P9" s="11" t="s">
+      <c r="Q9" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="Q9" s="11" t="s">
+      <c r="R9" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="S9" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="R9" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="S9" s="11" t="s">
+      <c r="T9" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="T9" s="11" t="s">
+      <c r="U9" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="U9" s="11" t="s">
+      <c r="V9" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="V9" s="11" t="s">
+      <c r="W9" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="W9" s="11" t="s">
+      <c r="X9" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="X9" s="11" t="s">
-        <v>116</v>
-      </c>
       <c r="Y9" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="Z9" s="4"/>
     </row>
@@ -1673,7 +1682,7 @@
         <v>2</v>
       </c>
       <c r="I10" s="47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>67</v>
@@ -1695,7 +1704,7 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" t="s">
@@ -1717,7 +1726,7 @@
         <v>2</v>
       </c>
       <c r="I11" s="47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>67</v>
@@ -1729,25 +1738,25 @@
         <v>36</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N11" s="9" t="s">
         <v>37</v>
       </c>
       <c r="O11" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P11" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q11" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R11" s="18" t="s">
         <v>44</v>
       </c>
       <c r="S11" s="25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="T11" s="32" t="s">
         <v>41</v>
@@ -1768,10 +1777,10 @@
     </row>
     <row r="12" spans="1:26" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="53" t="s">
         <v>94</v>
-      </c>
-      <c r="C12" s="53" t="s">
-        <v>95</v>
       </c>
       <c r="D12" s="53" t="s">
         <v>70</v>
@@ -1780,16 +1789,16 @@
         <v>11</v>
       </c>
       <c r="F12" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" s="54" t="s">
         <v>96</v>
-      </c>
-      <c r="G12" s="54" t="s">
-        <v>97</v>
       </c>
       <c r="H12" s="51" t="s">
         <v>2</v>
       </c>
       <c r="I12" s="47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J12" s="51" t="s">
         <v>67</v>
@@ -1812,7 +1821,7 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C13" t="s">
         <v>48</v>
@@ -1833,7 +1842,7 @@
         <v>2</v>
       </c>
       <c r="I13" s="47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J13" s="9" t="s">
         <v>67</v>
@@ -1845,17 +1854,17 @@
         <v>36</v>
       </c>
       <c r="M13" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N13" s="38" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="O13" s="9"/>
       <c r="P13" s="9"/>
     </row>
     <row r="14" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>0</v>
@@ -1864,22 +1873,22 @@
         <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E14" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>110</v>
-      </c>
       <c r="H14" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>16</v>
@@ -1906,13 +1915,13 @@
         <v>46</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="8"/>
@@ -1929,16 +1938,16 @@
     </row>
     <row r="16" spans="1:26" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A16" s="53" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B16" s="55" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C16" s="40" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E16" s="56" t="s">
         <v>29</v>
@@ -1959,7 +1968,7 @@
     </row>
     <row r="17" spans="1:26" s="46" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>17</v>
@@ -1980,7 +1989,7 @@
         <v>8</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>15</v>
@@ -1989,13 +1998,13 @@
         <v>16</v>
       </c>
       <c r="K17" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="L17" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="M17" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>148</v>
       </c>
       <c r="N17" s="3"/>
       <c r="O17" s="37"/>
@@ -2013,34 +2022,34 @@
     </row>
     <row r="18" spans="1:26" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="53" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B18" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="47" t="s">
-        <v>83</v>
-      </c>
       <c r="D18" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="53" t="s">
         <v>74</v>
-      </c>
-      <c r="E18" s="53" t="s">
-        <v>75</v>
       </c>
       <c r="F18" s="51" t="s">
         <v>40</v>
       </c>
       <c r="G18" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="H18" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="H18" s="51" t="s">
+      <c r="I18" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="I18" s="51" t="s">
+      <c r="J18" s="47" t="s">
         <v>78</v>
-      </c>
-      <c r="J18" s="47" t="s">
-        <v>79</v>
       </c>
       <c r="K18" s="51"/>
       <c r="L18" s="51"/>
@@ -2051,7 +2060,7 @@
     </row>
     <row r="19" spans="1:26" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="53" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B19" s="47" t="s">
         <v>62</v>
@@ -2072,7 +2081,7 @@
         <v>50</v>
       </c>
       <c r="H19" s="47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I19" s="51" t="s">
         <v>67</v>
@@ -2095,7 +2104,7 @@
     </row>
     <row r="20" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>17</v>
@@ -2125,13 +2134,13 @@
         <v>15</v>
       </c>
       <c r="K20" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="L20" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="L20" s="3" t="s">
+      <c r="M20" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="M20" s="3" t="s">
-        <v>148</v>
       </c>
       <c r="N20" s="3"/>
       <c r="O20" s="37"/>
@@ -2152,7 +2161,7 @@
         <v>3</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C21" s="40">
         <v>22222020</v>
@@ -2193,7 +2202,7 @@
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -2216,10 +2225,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z23"/>
+  <dimension ref="A1:Z24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2240,7 +2249,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -2249,10 +2258,10 @@
         <v>17</v>
       </c>
       <c r="D1" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>130</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>131</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -2284,7 +2293,7 @@
         <v>46534534</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D2" s="31">
         <v>1161138551</v>
@@ -2298,7 +2307,7 @@
         <v>46534534</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E3" s="31">
         <v>1161138552</v>
@@ -2306,63 +2315,63 @@
     </row>
     <row r="4" spans="1:26" s="31" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B4" s="29">
         <v>46534534</v>
       </c>
       <c r="C4" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" s="32" t="s">
         <v>150</v>
-      </c>
-      <c r="D4" s="32" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:26" s="31" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B5" s="29">
         <v>46534534</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:26" s="31" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B6" s="29">
         <v>46534534</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:26" s="31" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B7" s="29">
         <v>46534534</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>0</v>
@@ -2403,10 +2412,10 @@
         <v>14</v>
       </c>
       <c r="D9" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="E9" s="20" t="s">
         <v>158</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:26" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2414,18 +2423,18 @@
         <v>51</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="11"/>
@@ -2453,7 +2462,7 @@
     </row>
     <row r="12" spans="1:26" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" s="49" t="s">
         <v>63</v>
@@ -2462,7 +2471,7 @@
     </row>
     <row r="13" spans="1:26" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B13" s="48">
         <v>38452795</v>
@@ -2471,16 +2480,16 @@
     </row>
     <row r="14" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>136</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>137</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="5"/>
@@ -2507,7 +2516,7 @@
     </row>
     <row r="15" spans="1:26" s="40" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B15" s="49" t="s">
         <v>63</v>
@@ -2557,7 +2566,7 @@
     </row>
     <row r="17" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>0</v>
@@ -2589,15 +2598,15 @@
     </row>
     <row r="18" spans="1:26" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>0</v>
@@ -2629,15 +2638,15 @@
     </row>
     <row r="20" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>71</v>
+        <v>188</v>
       </c>
     </row>
     <row r="21" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>0</v>
@@ -2669,15 +2678,51 @@
     </row>
     <row r="22" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B22" s="41" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="41"/>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+      <c r="U23" s="4"/>
+      <c r="V23" s="4"/>
+      <c r="W23" s="4"/>
+      <c r="X23" s="4"/>
+      <c r="Y23" s="4"/>
+      <c r="Z23" s="4"/>
+    </row>
+    <row r="24" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>183</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2689,8 +2734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2704,49 +2749,49 @@
   <sheetData>
     <row r="1" spans="1:27" s="46" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>110</v>
-      </c>
       <c r="O1" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="P1" s="11"/>
       <c r="Q1" s="11"/>
@@ -2763,25 +2808,25 @@
     </row>
     <row r="2" spans="1:27" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" s="31" t="s">
         <v>63</v>
       </c>
       <c r="C2" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="29" t="s">
-        <v>156</v>
-      </c>
-      <c r="E2" s="33" t="s">
+      <c r="F2" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="32" t="s">
         <v>88</v>
-      </c>
-      <c r="F2" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="G2" s="32" t="s">
-        <v>89</v>
       </c>
       <c r="H2" s="32" t="s">
         <v>41</v>
@@ -2802,7 +2847,7 @@
         <v>21</v>
       </c>
       <c r="N2" s="30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O2" s="32" t="s">
         <v>44</v>
@@ -2816,10 +2861,10 @@
         <v>63</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E3" s="32"/>
       <c r="F3" s="32"/>
@@ -2830,25 +2875,25 @@
     </row>
     <row r="4" spans="1:27" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" s="31" t="s">
         <v>63</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G4" s="32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H4" s="31">
         <v>1</v>
@@ -2857,7 +2902,7 @@
         <v>2019</v>
       </c>
       <c r="J4" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K4" s="31" t="s">
         <v>22</v>
@@ -2866,12 +2911,12 @@
         <v>19784521</v>
       </c>
       <c r="M4" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:27" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>0</v>
@@ -2888,10 +2933,10 @@
         <v>32</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="19"/>
@@ -2901,17 +2946,17 @@
         <v>33</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="19"/>
     </row>
     <row r="8" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>0</v>
@@ -2920,40 +2965,40 @@
         <v>17</v>
       </c>
       <c r="D8" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="G8" s="11" t="s">
+      <c r="I8" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="H8" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="I8" s="11" t="s">
+      <c r="J8" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="K8" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="L8" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="L8" s="11" t="s">
+      <c r="M8" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="M8" s="11" t="s">
+      <c r="N8" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="N8" s="11" t="s">
-        <v>116</v>
-      </c>
       <c r="O8" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
@@ -2970,23 +3015,23 @@
     </row>
     <row r="9" spans="1:27" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H9" s="18" t="s">
         <v>44</v>
@@ -2994,23 +3039,23 @@
     </row>
     <row r="10" spans="1:27" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H10" s="18" t="s">
         <v>44</v>
@@ -3026,7 +3071,7 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B11">
         <v>18766558</v>
@@ -3035,42 +3080,42 @@
         <v>45</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H11" s="18" t="s">
         <v>44</v>
       </c>
       <c r="I11" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="J11" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="J11" s="32" t="s">
+      <c r="K11" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="L11" s="32" t="s">
         <v>182</v>
-      </c>
-      <c r="K11" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="L11" s="32" t="s">
-        <v>183</v>
       </c>
       <c r="M11" s="18" t="s">
         <v>22</v>
       </c>
       <c r="N11" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O11" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>0</v>
@@ -3079,37 +3124,37 @@
         <v>17</v>
       </c>
       <c r="D12" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="F12" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="G12" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="H12" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="G12" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="H12" s="11" t="s">
+      <c r="I12" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="J12" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="J12" s="11" t="s">
+      <c r="K12" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="K12" s="11" t="s">
+      <c r="L12" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="L12" s="11" t="s">
+      <c r="M12" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="M12" s="11" t="s">
-        <v>116</v>
-      </c>
       <c r="N12" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O12" s="11"/>
       <c r="P12" s="4"/>
@@ -3127,13 +3172,13 @@
     </row>
     <row r="13" spans="1:27" s="31" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B13" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="C13" s="29" t="s">
         <v>185</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>186</v>
       </c>
       <c r="D13" s="30"/>
       <c r="F13" s="30"/>
@@ -3149,13 +3194,13 @@
     </row>
     <row r="14" spans="1:27" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D14" s="30"/>
       <c r="F14" s="30"/>
@@ -3171,28 +3216,28 @@
     </row>
     <row r="15" spans="1:27" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F15" s="30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G15" s="32" t="s">
         <v>44</v>
       </c>
       <c r="H15" s="32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I15" s="32" t="s">
         <v>41</v>
@@ -3210,13 +3255,13 @@
         <v>63</v>
       </c>
       <c r="N15" s="34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O15" s="34"/>
     </row>
     <row r="16" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>0</v>
@@ -3225,37 +3270,37 @@
         <v>17</v>
       </c>
       <c r="D16" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="F16" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="G16" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="H16" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="G16" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="H16" s="11" t="s">
+      <c r="I16" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="I16" s="11" t="s">
+      <c r="J16" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="J16" s="11" t="s">
+      <c r="K16" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="K16" s="11" t="s">
+      <c r="L16" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="L16" s="11" t="s">
+      <c r="M16" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="M16" s="11" t="s">
-        <v>116</v>
-      </c>
       <c r="N16" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O16" s="11"/>
       <c r="P16" s="4"/>
@@ -3276,10 +3321,10 @@
         <v>25</v>
       </c>
       <c r="B17" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="C17" s="29" t="s">
         <v>185</v>
-      </c>
-      <c r="C17" s="29" t="s">
-        <v>186</v>
       </c>
       <c r="D17" s="55"/>
     </row>
@@ -3291,34 +3336,34 @@
         <v>63</v>
       </c>
       <c r="C18" s="55" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D18" s="55"/>
     </row>
     <row r="19" spans="1:14" s="40" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="58" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B19" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="C19" s="29" t="s">
         <v>185</v>
       </c>
-      <c r="C19" s="29" t="s">
-        <v>186</v>
-      </c>
       <c r="D19" s="30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E19" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F19" s="30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G19" s="32" t="s">
         <v>44</v>
       </c>
       <c r="H19" s="59" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I19" s="32" t="s">
         <v>41</v>
@@ -3336,7 +3381,7 @@
         <v>69</v>
       </c>
       <c r="N19" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -3363,7 +3408,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cuentas y ventas equipo
</commit_message>
<xml_diff>
--- a/E2ESIT.xlsx
+++ b/E2ESIT.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="197">
   <si>
     <t>N.º Documento</t>
   </si>
@@ -435,9 +435,6 @@
   </si>
   <si>
     <t>1544</t>
-  </si>
-  <si>
-    <t>666</t>
   </si>
   <si>
     <t>Calle</t>
@@ -1302,8 +1299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1355,13 +1352,13 @@
         <v>16</v>
       </c>
       <c r="K1" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="N1" s="10" t="s">
         <v>101</v>
@@ -1428,7 +1425,7 @@
         <v>14</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>35</v>
@@ -1478,7 +1475,7 @@
         <v>14</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K3" s="9" t="s">
         <v>35</v>
@@ -1640,7 +1637,7 @@
         <v>103</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>129</v>
@@ -1669,7 +1666,7 @@
         <v>69</v>
       </c>
       <c r="B7" s="93" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C7" s="40" t="s">
         <v>2</v>
@@ -1681,7 +1678,7 @@
         <v>115</v>
       </c>
       <c r="F7" s="32" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G7" s="32" t="s">
         <v>43</v>
@@ -1703,7 +1700,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="93" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C8" s="40" t="s">
         <v>2</v>
@@ -1746,7 +1743,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>15</v>
@@ -1755,13 +1752,13 @@
         <v>16</v>
       </c>
       <c r="L9" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="M9" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="N9" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="O9" s="10" t="s">
         <v>101</v>
@@ -1828,7 +1825,7 @@
         <v>14</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L10" s="8" t="s">
         <v>35</v>
@@ -1875,7 +1872,7 @@
         <v>14</v>
       </c>
       <c r="L11" s="39" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M11" s="39" t="s">
         <v>35</v>
@@ -1946,7 +1943,7 @@
         <v>14</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L12" s="47"/>
       <c r="M12" s="51"/>
@@ -1990,16 +1987,16 @@
         <v>14</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L13" s="8" t="s">
         <v>35</v>
       </c>
       <c r="M13" s="9" t="s">
-        <v>138</v>
+        <v>36</v>
       </c>
       <c r="N13" s="38" t="s">
-        <v>138</v>
+        <v>36</v>
       </c>
       <c r="O13" s="9"/>
       <c r="P13" s="9"/>
@@ -2015,7 +2012,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>101</v>
@@ -2027,7 +2024,7 @@
         <v>103</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>129</v>
@@ -2056,8 +2053,8 @@
       <c r="A15" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="88" t="s">
-        <v>187</v>
+      <c r="B15" s="93" t="s">
+        <v>196</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>2</v>
@@ -2082,8 +2079,8 @@
       <c r="A16" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="B16" s="88" t="s">
-        <v>187</v>
+      <c r="B16" s="93" t="s">
+        <v>196</v>
       </c>
       <c r="C16" s="40" t="s">
         <v>2</v>
@@ -2110,7 +2107,7 @@
     </row>
     <row r="17" spans="1:26" s="46" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>17</v>
@@ -2131,7 +2128,7 @@
         <v>8</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>15</v>
@@ -2140,13 +2137,13 @@
         <v>16</v>
       </c>
       <c r="K17" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="L17" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="M17" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="N17" s="3"/>
       <c r="O17" s="37"/>
@@ -2164,10 +2161,10 @@
     </row>
     <row r="18" spans="1:26" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="53" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B18" s="88" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C18" s="47" t="s">
         <v>77</v>
@@ -2202,7 +2199,7 @@
     </row>
     <row r="19" spans="1:26" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="53" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B19" s="47" t="s">
         <v>61</v>
@@ -2229,7 +2226,7 @@
         <v>14</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K19" s="47" t="s">
         <v>35</v>
@@ -2246,7 +2243,7 @@
     </row>
     <row r="20" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>17</v>
@@ -2276,13 +2273,13 @@
         <v>15</v>
       </c>
       <c r="K20" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="L20" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L20" s="3" t="s">
+      <c r="M20" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="M20" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="N20" s="3"/>
       <c r="O20" s="37"/>
@@ -2303,7 +2300,7 @@
         <v>3</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C21" s="40">
         <v>22222020</v>
@@ -2327,7 +2324,7 @@
         <v>14</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K21" s="51" t="s">
         <v>35</v>
@@ -2350,7 +2347,7 @@
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2441,7 +2438,7 @@
         <v>46534534</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D2" s="31">
         <v>1161138551</v>
@@ -2455,7 +2452,7 @@
         <v>46534534</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E3" s="31">
         <v>1161138552</v>
@@ -2463,56 +2460,56 @@
     </row>
     <row r="4" spans="1:26" s="31" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B4" s="29">
         <v>46534534</v>
       </c>
       <c r="C4" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="32" t="s">
         <v>143</v>
-      </c>
-      <c r="D4" s="32" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:26" s="31" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B5" s="29">
         <v>46534534</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:26" s="83" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B6" s="29">
         <v>46534534</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E6" s="84"/>
     </row>
     <row r="7" spans="1:26" s="31" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B7" s="29">
         <v>46534534</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D7" s="32" t="s">
         <v>72</v>
@@ -2520,13 +2517,13 @@
     </row>
     <row r="8" spans="1:26" s="31" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="31" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B8" s="81">
         <v>46534534</v>
       </c>
       <c r="C8" s="81" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -2563,7 +2560,7 @@
     </row>
     <row r="10" spans="1:26" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>62</v>
@@ -2572,10 +2569,10 @@
         <v>14</v>
       </c>
       <c r="D10" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="E10" s="20" t="s">
         <v>151</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:26" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2583,7 +2580,7 @@
         <v>50</v>
       </c>
       <c r="B11" s="50" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -2676,7 +2673,7 @@
     </row>
     <row r="16" spans="1:26" s="40" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B16" s="49" t="s">
         <v>62</v>
@@ -2712,7 +2709,7 @@
     </row>
     <row r="17" spans="1:26" s="40" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="42" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B17" s="49" t="s">
         <v>62</v>
@@ -2748,7 +2745,7 @@
     </row>
     <row r="18" spans="1:26" s="40" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="42" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B18" s="49" t="s">
         <v>62</v>
@@ -2829,12 +2826,12 @@
         <v>94</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>0</v>
@@ -2866,15 +2863,15 @@
     </row>
     <row r="23" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B23" s="41" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>0</v>
@@ -2906,15 +2903,15 @@
     </row>
     <row r="25" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B25" s="41" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>0</v>
@@ -2946,10 +2943,10 @@
     </row>
     <row r="27" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -3047,7 +3044,7 @@
         <v>81</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E2" s="33" t="s">
         <v>82</v>
@@ -3094,7 +3091,7 @@
         <v>68</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E3" s="32"/>
       <c r="F3" s="32"/>
@@ -3114,7 +3111,7 @@
         <v>81</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E4" s="32" t="s">
         <v>116</v>
@@ -3163,7 +3160,7 @@
         <v>32</v>
       </c>
       <c r="B6" s="88" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>95</v>
@@ -3176,7 +3173,7 @@
         <v>33</v>
       </c>
       <c r="B7" s="88" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>110</v>
@@ -3245,16 +3242,16 @@
     </row>
     <row r="9" spans="1:27" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B9" s="61" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C9" s="62" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D9" s="64" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E9" s="65" t="s">
         <v>82</v>
@@ -3271,16 +3268,16 @@
     </row>
     <row r="10" spans="1:27" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B10" s="66" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C10" s="67" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D10" s="69" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E10" s="70" t="s">
         <v>82</v>
@@ -3305,13 +3302,13 @@
     </row>
     <row r="11" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A11" s="76" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B11" s="79" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C11" s="81" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D11" s="74" t="s">
         <v>44</v>
@@ -3329,25 +3326,25 @@
         <v>43</v>
       </c>
       <c r="I11" s="77" t="s">
+        <v>169</v>
+      </c>
+      <c r="J11" s="78" t="s">
         <v>170</v>
-      </c>
-      <c r="J11" s="78" t="s">
-        <v>171</v>
       </c>
       <c r="K11" s="78" t="s">
         <v>73</v>
       </c>
       <c r="L11" s="78" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M11" s="73" t="s">
         <v>22</v>
       </c>
       <c r="N11" s="72" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O11" s="72" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="P11" s="71"/>
       <c r="Q11" s="71"/>
@@ -3424,10 +3421,10 @@
         <v>97</v>
       </c>
       <c r="B13" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="C13" s="29" t="s">
         <v>174</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>175</v>
       </c>
       <c r="D13" s="30"/>
       <c r="F13" s="30"/>
@@ -3443,13 +3440,13 @@
     </row>
     <row r="14" spans="1:27" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B14" s="72" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C14" s="67" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D14" s="30"/>
       <c r="F14" s="30"/>
@@ -3468,13 +3465,13 @@
         <v>96</v>
       </c>
       <c r="B15" s="87" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C15" s="81" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E15" s="31" t="s">
         <v>29</v>
@@ -3483,7 +3480,7 @@
         <v>30</v>
       </c>
       <c r="G15" s="31" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H15" s="82" t="s">
         <v>82</v>
@@ -3590,10 +3587,10 @@
         <v>25</v>
       </c>
       <c r="B17" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="C17" s="29" t="s">
         <v>174</v>
-      </c>
-      <c r="C17" s="29" t="s">
-        <v>175</v>
       </c>
       <c r="D17" s="55"/>
     </row>
@@ -3605,7 +3602,7 @@
         <v>62</v>
       </c>
       <c r="C18" s="55" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D18" s="55"/>
     </row>
@@ -3614,10 +3611,10 @@
         <v>120</v>
       </c>
       <c r="B19" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="C19" s="29" t="s">
         <v>174</v>
-      </c>
-      <c r="C19" s="29" t="s">
-        <v>175</v>
       </c>
       <c r="D19" s="30" t="s">
         <v>82</v>
@@ -3677,7 +3674,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cuentas y gestiones agente
</commit_message>
<xml_diff>
--- a/E2ESIT.xlsx
+++ b/E2ESIT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Altas y Nominacion" sheetId="8" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="200">
   <si>
     <t>N.º Documento</t>
   </si>
@@ -612,6 +612,15 @@
   </si>
   <si>
     <t>2222203</t>
+  </si>
+  <si>
+    <t>Gestion Consulta de Saldo</t>
+  </si>
+  <si>
+    <t>SaldoConsulta</t>
+  </si>
+  <si>
+    <t>1 - CFT %0.0</t>
   </si>
 </sst>
 </file>
@@ -1299,7 +1308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -2370,10 +2379,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z27"/>
+  <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2786,7 +2795,9 @@
       <c r="B19" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="18"/>
+      <c r="C19" s="18" t="s">
+        <v>148</v>
+      </c>
       <c r="D19" s="18"/>
     </row>
     <row r="20" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -2949,6 +2960,46 @@
         <v>172</v>
       </c>
     </row>
+    <row r="28" spans="1:26" s="71" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="4"/>
+      <c r="W28" s="4"/>
+      <c r="X28" s="4"/>
+      <c r="Y28" s="4"/>
+      <c r="Z28" s="4"/>
+    </row>
+    <row r="29" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="B29">
+        <v>15907314</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2959,8 +3010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15:G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3077,7 +3128,7 @@
         <v>87</v>
       </c>
       <c r="O2" s="32" t="s">
-        <v>43</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:27" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -3586,11 +3637,11 @@
       <c r="A17" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="28" t="s">
-        <v>173</v>
-      </c>
-      <c r="C17" s="29" t="s">
-        <v>174</v>
+      <c r="B17" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="55" t="s">
+        <v>148</v>
       </c>
       <c r="D17" s="55"/>
     </row>
@@ -3598,11 +3649,11 @@
       <c r="A18" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="55" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" s="55" t="s">
-        <v>148</v>
+      <c r="B18" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="C18" s="81" t="s">
+        <v>174</v>
       </c>
       <c r="D18" s="55"/>
     </row>
@@ -3626,7 +3677,7 @@
         <v>87</v>
       </c>
       <c r="G19" s="32" t="s">
-        <v>43</v>
+        <v>199</v>
       </c>
       <c r="H19" s="59" t="s">
         <v>98</v>
@@ -3672,6 +3723,10 @@
       <c r="M21" s="16"/>
       <c r="N21" s="16"/>
     </row>
+    <row r="23" spans="1:14" ht="15" x14ac:dyDescent="0.35">
+      <c r="B23" s="28"/>
+      <c r="C23" s="81"/>
+    </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>152</v>

</xml_diff>

<commit_message>
una linea pa el nico
</commit_message>
<xml_diff>
--- a/E2ESIT.xlsx
+++ b/E2ESIT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Altas y Nominacion" sheetId="8" r:id="rId1"/>
@@ -515,9 +515,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>341309797</t>
-  </si>
-  <si>
     <t>10777540</t>
   </si>
   <si>
@@ -621,6 +618,9 @@
   </si>
   <si>
     <t>1 - CFT %0.0</t>
+  </si>
+  <si>
+    <t>9090909090</t>
   </si>
 </sst>
 </file>
@@ -1308,8 +1308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1434,7 +1434,7 @@
         <v>14</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>35</v>
@@ -1484,7 +1484,7 @@
         <v>14</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K3" s="9" t="s">
         <v>35</v>
@@ -1675,7 +1675,7 @@
         <v>69</v>
       </c>
       <c r="B7" s="93" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C7" s="40" t="s">
         <v>2</v>
@@ -1709,7 +1709,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="93" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C8" s="40" t="s">
         <v>2</v>
@@ -1834,7 +1834,7 @@
         <v>14</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L10" s="8" t="s">
         <v>35</v>
@@ -1881,7 +1881,7 @@
         <v>14</v>
       </c>
       <c r="L11" s="39" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M11" s="39" t="s">
         <v>35</v>
@@ -1952,7 +1952,7 @@
         <v>14</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L12" s="47"/>
       <c r="M12" s="51"/>
@@ -1996,7 +1996,7 @@
         <v>14</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L13" s="8" t="s">
         <v>35</v>
@@ -2063,7 +2063,7 @@
         <v>45</v>
       </c>
       <c r="B15" s="93" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>2</v>
@@ -2089,7 +2089,7 @@
         <v>75</v>
       </c>
       <c r="B16" s="93" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C16" s="40" t="s">
         <v>2</v>
@@ -2173,7 +2173,7 @@
         <v>160</v>
       </c>
       <c r="B18" s="88" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C18" s="47" t="s">
         <v>77</v>
@@ -2235,7 +2235,7 @@
         <v>14</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K19" s="47" t="s">
         <v>35</v>
@@ -2308,8 +2308,8 @@
       <c r="A21" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="51" t="s">
-        <v>164</v>
+      <c r="B21" s="93" t="s">
+        <v>199</v>
       </c>
       <c r="C21" s="40">
         <v>22222020</v>
@@ -2333,7 +2333,7 @@
         <v>14</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K21" s="51" t="s">
         <v>35</v>
@@ -2526,7 +2526,7 @@
     </row>
     <row r="8" spans="1:26" s="31" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="31" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B8" s="81">
         <v>46534534</v>
@@ -2569,7 +2569,7 @@
     </row>
     <row r="10" spans="1:26" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>62</v>
@@ -2589,7 +2589,7 @@
         <v>50</v>
       </c>
       <c r="B11" s="50" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -2718,7 +2718,7 @@
     </row>
     <row r="17" spans="1:26" s="40" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="42" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B17" s="49" t="s">
         <v>62</v>
@@ -2754,7 +2754,7 @@
     </row>
     <row r="18" spans="1:26" s="40" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="42" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B18" s="49" t="s">
         <v>62</v>
@@ -2837,12 +2837,12 @@
         <v>94</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>0</v>
@@ -2877,12 +2877,12 @@
         <v>153</v>
       </c>
       <c r="B23" s="41" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>0</v>
@@ -2917,12 +2917,12 @@
         <v>154</v>
       </c>
       <c r="B25" s="41" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>0</v>
@@ -2954,15 +2954,15 @@
     </row>
     <row r="27" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:26" s="71" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>0</v>
@@ -2994,7 +2994,7 @@
     </row>
     <row r="29" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B29">
         <v>15907314</v>
@@ -3010,7 +3010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -3128,7 +3128,7 @@
         <v>87</v>
       </c>
       <c r="O2" s="32" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:27" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -3211,7 +3211,7 @@
         <v>32</v>
       </c>
       <c r="B6" s="88" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>95</v>
@@ -3224,7 +3224,7 @@
         <v>33</v>
       </c>
       <c r="B7" s="88" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>110</v>
@@ -3293,16 +3293,16 @@
     </row>
     <row r="9" spans="1:27" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B9" s="61" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C9" s="62" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D9" s="64" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E9" s="65" t="s">
         <v>82</v>
@@ -3319,16 +3319,16 @@
     </row>
     <row r="10" spans="1:27" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B10" s="66" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C10" s="67" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D10" s="69" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E10" s="70" t="s">
         <v>82</v>
@@ -3353,13 +3353,13 @@
     </row>
     <row r="11" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A11" s="76" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B11" s="79" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C11" s="81" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D11" s="74" t="s">
         <v>44</v>
@@ -3377,16 +3377,16 @@
         <v>43</v>
       </c>
       <c r="I11" s="77" t="s">
+        <v>168</v>
+      </c>
+      <c r="J11" s="78" t="s">
         <v>169</v>
-      </c>
-      <c r="J11" s="78" t="s">
-        <v>170</v>
       </c>
       <c r="K11" s="78" t="s">
         <v>73</v>
       </c>
       <c r="L11" s="78" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M11" s="73" t="s">
         <v>22</v>
@@ -3395,7 +3395,7 @@
         <v>149</v>
       </c>
       <c r="O11" s="72" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="P11" s="71"/>
       <c r="Q11" s="71"/>
@@ -3472,10 +3472,10 @@
         <v>97</v>
       </c>
       <c r="B13" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="C13" s="29" t="s">
         <v>173</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>174</v>
       </c>
       <c r="D13" s="30"/>
       <c r="F13" s="30"/>
@@ -3494,10 +3494,10 @@
         <v>156</v>
       </c>
       <c r="B14" s="72" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C14" s="67" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D14" s="30"/>
       <c r="F14" s="30"/>
@@ -3516,13 +3516,13 @@
         <v>96</v>
       </c>
       <c r="B15" s="87" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C15" s="81" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E15" s="31" t="s">
         <v>29</v>
@@ -3531,7 +3531,7 @@
         <v>30</v>
       </c>
       <c r="G15" s="31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H15" s="82" t="s">
         <v>82</v>
@@ -3650,10 +3650,10 @@
         <v>26</v>
       </c>
       <c r="B18" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="C18" s="81" t="s">
         <v>173</v>
-      </c>
-      <c r="C18" s="81" t="s">
-        <v>174</v>
       </c>
       <c r="D18" s="55"/>
     </row>
@@ -3662,10 +3662,10 @@
         <v>120</v>
       </c>
       <c r="B19" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="C19" s="29" t="s">
         <v>173</v>
-      </c>
-      <c r="C19" s="29" t="s">
-        <v>174</v>
       </c>
       <c r="D19" s="30" t="s">
         <v>82</v>
@@ -3677,7 +3677,7 @@
         <v>87</v>
       </c>
       <c r="G19" s="32" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H19" s="59" t="s">
         <v>98</v>

</xml_diff>